<commit_message>
analysis for the antag screen done with e cells
</commit_message>
<xml_diff>
--- a/Kamarck Ecell Transfections 2-16.xlsx
+++ b/Kamarck Ecell Transfections 2-16.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/mainland/Projects/TAARs/E cell Optimization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/storage/mainland/Projects/TAARs/E cell Optimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1650,7 +1650,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="293">
+  <cellXfs count="294">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -2013,6 +2013,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2023,6 +2024,16 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2062,16 +2073,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2511,20 +2512,20 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="272" t="s">
+      <c r="B1" s="273" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="273"/>
-      <c r="D1" s="273"/>
-      <c r="E1" s="273"/>
-      <c r="F1" s="273"/>
-      <c r="G1" s="273"/>
-      <c r="H1" s="273"/>
-      <c r="I1" s="273"/>
-      <c r="J1" s="273"/>
-      <c r="K1" s="273"/>
-      <c r="L1" s="273"/>
-      <c r="M1" s="274"/>
+      <c r="C1" s="274"/>
+      <c r="D1" s="274"/>
+      <c r="E1" s="274"/>
+      <c r="F1" s="274"/>
+      <c r="G1" s="274"/>
+      <c r="H1" s="274"/>
+      <c r="I1" s="274"/>
+      <c r="J1" s="274"/>
+      <c r="K1" s="274"/>
+      <c r="L1" s="274"/>
+      <c r="M1" s="275"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
     </row>
@@ -3029,10 +3030,10 @@
         <f>1/96</f>
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="G17" s="275" t="s">
+      <c r="G17" s="276" t="s">
         <v>75</v>
       </c>
-      <c r="H17" s="275"/>
+      <c r="H17" s="276"/>
       <c r="I17" s="114" t="s">
         <v>76</v>
       </c>
@@ -4181,8 +4182,8 @@
   </sheetPr>
   <dimension ref="A1:Y132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="AA7" sqref="AA7"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="L90" sqref="L90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4191,20 +4192,20 @@
       <c r="A1" s="134" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="280" t="s">
+      <c r="B1" s="285" t="s">
         <v>232</v>
       </c>
-      <c r="C1" s="281"/>
-      <c r="D1" s="281"/>
-      <c r="E1" s="281"/>
-      <c r="F1" s="281"/>
-      <c r="G1" s="281"/>
-      <c r="H1" s="281"/>
-      <c r="I1" s="281"/>
-      <c r="J1" s="281"/>
-      <c r="K1" s="281"/>
-      <c r="L1" s="281"/>
-      <c r="M1" s="282"/>
+      <c r="C1" s="286"/>
+      <c r="D1" s="286"/>
+      <c r="E1" s="286"/>
+      <c r="F1" s="286"/>
+      <c r="G1" s="286"/>
+      <c r="H1" s="286"/>
+      <c r="I1" s="286"/>
+      <c r="J1" s="286"/>
+      <c r="K1" s="286"/>
+      <c r="L1" s="286"/>
+      <c r="M1" s="287"/>
     </row>
     <row r="2" spans="1:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="135" t="s">
@@ -4227,9 +4228,9 @@
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
-      <c r="M2" s="283"/>
-      <c r="N2" s="283"/>
-      <c r="O2" s="283"/>
+      <c r="M2" s="288"/>
+      <c r="N2" s="288"/>
+      <c r="O2" s="288"/>
     </row>
     <row r="3" spans="1:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="141" t="s">
@@ -4244,16 +4245,16 @@
       <c r="G3" s="256">
         <v>1</v>
       </c>
-      <c r="H3" s="284" t="s">
+      <c r="H3" s="289" t="s">
         <v>91</v>
       </c>
-      <c r="I3" s="273"/>
-      <c r="J3" s="273"/>
-      <c r="K3" s="274"/>
+      <c r="I3" s="274"/>
+      <c r="J3" s="274"/>
+      <c r="K3" s="275"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="283"/>
-      <c r="N3" s="283"/>
-      <c r="O3" s="283"/>
+      <c r="M3" s="288"/>
+      <c r="N3" s="288"/>
+      <c r="O3" s="288"/>
     </row>
     <row r="4" spans="1:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="143" t="s">
@@ -4332,11 +4333,11 @@
         <f>(G5+0.2*G5)*1.11111111111111</f>
         <v>33.3333333333333</v>
       </c>
-      <c r="H6" s="285" t="s">
+      <c r="H6" s="290" t="s">
         <v>93</v>
       </c>
-      <c r="I6" s="286"/>
-      <c r="J6" s="287"/>
+      <c r="I6" s="291"/>
+      <c r="J6" s="292"/>
       <c r="K6" s="258"/>
       <c r="L6" s="3"/>
       <c r="M6" s="156" t="s">
@@ -4382,10 +4383,10 @@
       <c r="J7" s="133" t="s">
         <v>99</v>
       </c>
-      <c r="K7" s="288" t="s">
+      <c r="K7" s="293" t="s">
         <v>27</v>
       </c>
-      <c r="L7" s="288"/>
+      <c r="L7" s="293"/>
       <c r="M7" s="140" t="s">
         <v>100</v>
       </c>
@@ -5913,19 +5914,19 @@
         <f>((B58*D56)*0.25)+(B58*D56)</f>
         <v>484.375</v>
       </c>
-      <c r="G58" s="275" t="s">
+      <c r="G58" s="276" t="s">
         <v>75</v>
       </c>
-      <c r="H58" s="275"/>
+      <c r="H58" s="276"/>
       <c r="I58" s="133" t="s">
         <v>76</v>
       </c>
       <c r="J58" s="133"/>
       <c r="K58" s="133"/>
-      <c r="M58" s="275" t="s">
+      <c r="M58" s="276" t="s">
         <v>75</v>
       </c>
-      <c r="N58" s="275"/>
+      <c r="N58" s="276"/>
       <c r="O58" s="133" t="s">
         <v>76</v>
       </c>
@@ -6068,25 +6069,25 @@
       <c r="A66" s="247" t="s">
         <v>177</v>
       </c>
-      <c r="B66" s="276" t="s">
+      <c r="B66" s="281" t="s">
         <v>178</v>
       </c>
-      <c r="C66" s="276"/>
-      <c r="D66" s="277" t="s">
+      <c r="C66" s="281"/>
+      <c r="D66" s="282" t="s">
         <v>179</v>
       </c>
-      <c r="E66" s="277"/>
-      <c r="F66" s="278" t="s">
+      <c r="E66" s="282"/>
+      <c r="F66" s="283" t="s">
         <v>180</v>
       </c>
-      <c r="G66" s="278"/>
+      <c r="G66" s="283"/>
       <c r="H66" s="248" t="s">
         <v>181</v>
       </c>
       <c r="I66" s="249" t="s">
         <v>182</v>
       </c>
-      <c r="J66" s="279" t="s">
+      <c r="J66" s="284" t="s">
         <v>183</v>
       </c>
       <c r="K66" s="49"/>
@@ -6096,18 +6097,18 @@
       <c r="O66" s="247" t="s">
         <v>177</v>
       </c>
-      <c r="P66" s="276" t="s">
+      <c r="P66" s="281" t="s">
         <v>178</v>
       </c>
-      <c r="Q66" s="276"/>
-      <c r="R66" s="277" t="s">
+      <c r="Q66" s="281"/>
+      <c r="R66" s="282" t="s">
         <v>179</v>
       </c>
-      <c r="S66" s="277"/>
-      <c r="T66" s="278" t="s">
+      <c r="S66" s="282"/>
+      <c r="T66" s="283" t="s">
         <v>184</v>
       </c>
-      <c r="U66" s="278"/>
+      <c r="U66" s="283"/>
       <c r="V66" s="248" t="s">
         <v>181</v>
       </c>
@@ -6128,7 +6129,7 @@
       <c r="G67" s="250"/>
       <c r="H67" s="250"/>
       <c r="I67" s="250"/>
-      <c r="J67" s="279"/>
+      <c r="J67" s="284"/>
       <c r="K67" s="11"/>
       <c r="L67" s="11"/>
       <c r="M67" s="11"/>
@@ -6144,7 +6145,7 @@
       <c r="U67" s="250"/>
       <c r="V67" s="250"/>
       <c r="W67" s="250"/>
-      <c r="X67" s="279" t="s">
+      <c r="X67" s="284" t="s">
         <v>186</v>
       </c>
     </row>
@@ -6160,7 +6161,7 @@
       <c r="G68" s="250"/>
       <c r="H68" s="250"/>
       <c r="I68" s="251"/>
-      <c r="J68" s="279"/>
+      <c r="J68" s="284"/>
       <c r="K68" s="11"/>
       <c r="L68" s="11"/>
       <c r="M68" s="11"/>
@@ -6176,7 +6177,7 @@
       <c r="U68" s="250"/>
       <c r="V68" s="250"/>
       <c r="W68" s="251"/>
-      <c r="X68" s="279"/>
+      <c r="X68" s="284"/>
     </row>
     <row r="69" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A69" s="247" t="s">
@@ -6190,7 +6191,7 @@
       <c r="G69" s="250"/>
       <c r="H69" s="250"/>
       <c r="I69" s="251"/>
-      <c r="J69" s="279"/>
+      <c r="J69" s="284"/>
       <c r="K69" s="11"/>
       <c r="L69" s="11"/>
       <c r="M69" s="11"/>
@@ -6206,7 +6207,7 @@
       <c r="U69" s="250"/>
       <c r="V69" s="250"/>
       <c r="W69" s="251"/>
-      <c r="X69" s="279"/>
+      <c r="X69" s="284"/>
     </row>
     <row r="70" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A70" s="247" t="s">
@@ -6220,7 +6221,7 @@
       <c r="G70" s="250"/>
       <c r="H70" s="250"/>
       <c r="I70" s="251"/>
-      <c r="J70" s="279"/>
+      <c r="J70" s="284"/>
       <c r="K70" s="11"/>
       <c r="L70" s="11"/>
       <c r="M70" s="11"/>
@@ -6236,7 +6237,7 @@
       <c r="U70" s="250"/>
       <c r="V70" s="250"/>
       <c r="W70" s="251"/>
-      <c r="X70" s="279"/>
+      <c r="X70" s="284"/>
     </row>
     <row r="71" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A71" s="247" t="s">
@@ -6250,7 +6251,7 @@
       <c r="G71" s="250"/>
       <c r="H71" s="250"/>
       <c r="I71" s="251"/>
-      <c r="J71" s="279"/>
+      <c r="J71" s="284"/>
       <c r="K71" s="11"/>
       <c r="L71" s="11"/>
       <c r="M71" s="11"/>
@@ -6266,7 +6267,7 @@
       <c r="U71" s="250"/>
       <c r="V71" s="250"/>
       <c r="W71" s="251"/>
-      <c r="X71" s="279"/>
+      <c r="X71" s="284"/>
     </row>
     <row r="72" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A72" s="247" t="s">
@@ -6658,1145 +6659,1145 @@
       <c r="A94" s="247" t="s">
         <v>177</v>
       </c>
-      <c r="B94" s="291" t="s">
+      <c r="B94" s="279" t="s">
         <v>178</v>
       </c>
-      <c r="C94" s="291"/>
-      <c r="D94" s="291"/>
-      <c r="E94" s="291"/>
-      <c r="F94" s="291"/>
-      <c r="G94" s="291"/>
-      <c r="H94" s="291" t="s">
+      <c r="C94" s="279"/>
+      <c r="D94" s="279"/>
+      <c r="E94" s="279"/>
+      <c r="F94" s="279"/>
+      <c r="G94" s="279"/>
+      <c r="H94" s="279" t="s">
         <v>179</v>
       </c>
-      <c r="I94" s="291"/>
-      <c r="J94" s="291"/>
-      <c r="K94" s="291"/>
-      <c r="L94" s="291"/>
-      <c r="M94" s="291"/>
-      <c r="N94" s="289" t="s">
+      <c r="I94" s="279"/>
+      <c r="J94" s="279"/>
+      <c r="K94" s="279"/>
+      <c r="L94" s="279"/>
+      <c r="M94" s="279"/>
+      <c r="N94" s="277" t="s">
         <v>180</v>
       </c>
-      <c r="O94" s="289"/>
-      <c r="P94" s="289"/>
-      <c r="Q94" s="289"/>
-      <c r="R94" s="289"/>
-      <c r="S94" s="289"/>
-      <c r="T94" s="289" t="s">
+      <c r="O94" s="277"/>
+      <c r="P94" s="277"/>
+      <c r="Q94" s="277"/>
+      <c r="R94" s="277"/>
+      <c r="S94" s="277"/>
+      <c r="T94" s="277" t="s">
         <v>181</v>
       </c>
-      <c r="U94" s="289"/>
-      <c r="V94" s="289"/>
-      <c r="W94" s="289" t="s">
+      <c r="U94" s="277"/>
+      <c r="V94" s="277"/>
+      <c r="W94" s="277" t="s">
         <v>182</v>
       </c>
-      <c r="X94" s="289"/>
-      <c r="Y94" s="289"/>
+      <c r="X94" s="277"/>
+      <c r="Y94" s="277"/>
     </row>
     <row r="95" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A95" s="247" t="s">
         <v>185</v>
       </c>
-      <c r="B95" s="133">
-        <v>903</v>
-      </c>
-      <c r="C95" s="133">
-        <v>809</v>
-      </c>
-      <c r="D95" s="133">
-        <v>911</v>
-      </c>
-      <c r="E95" s="133">
-        <v>817</v>
-      </c>
-      <c r="F95" s="133">
-        <v>919</v>
-      </c>
-      <c r="G95" s="133">
-        <v>825</v>
-      </c>
-      <c r="H95" s="133">
-        <v>927</v>
-      </c>
-      <c r="I95" s="133">
-        <v>833</v>
-      </c>
-      <c r="J95" s="133">
-        <v>935</v>
-      </c>
-      <c r="K95" s="292" t="s">
+      <c r="B95" s="272">
+        <v>1217</v>
+      </c>
+      <c r="C95" s="272">
+        <v>1125</v>
+      </c>
+      <c r="D95" s="272">
+        <v>1225</v>
+      </c>
+      <c r="E95" s="272">
+        <v>1133</v>
+      </c>
+      <c r="F95" s="272">
+        <v>1233</v>
+      </c>
+      <c r="G95" s="272">
+        <v>1141</v>
+      </c>
+      <c r="H95" s="272">
+        <v>1241</v>
+      </c>
+      <c r="I95" s="272">
+        <v>1149</v>
+      </c>
+      <c r="J95" s="272">
+        <v>1249</v>
+      </c>
+      <c r="K95" s="280" t="s">
         <v>237</v>
       </c>
-      <c r="L95" s="292"/>
-      <c r="M95" s="292"/>
-      <c r="N95" s="133">
-        <v>841</v>
-      </c>
-      <c r="O95" s="133">
-        <v>943</v>
-      </c>
-      <c r="P95" s="133">
-        <v>849</v>
-      </c>
-      <c r="Q95" s="133">
-        <v>951</v>
-      </c>
-      <c r="R95" s="133">
-        <v>857</v>
-      </c>
-      <c r="S95" s="133">
-        <v>959</v>
+      <c r="L95" s="280"/>
+      <c r="M95" s="280"/>
+      <c r="N95" s="272">
+        <v>1157</v>
+      </c>
+      <c r="O95" s="272">
+        <v>1257</v>
+      </c>
+      <c r="P95" s="272">
+        <v>1165</v>
+      </c>
+      <c r="Q95" s="272">
+        <v>1265</v>
+      </c>
+      <c r="R95" s="272">
+        <v>1173</v>
+      </c>
+      <c r="S95" s="272">
+        <v>1273</v>
       </c>
       <c r="T95" s="150">
-        <v>481</v>
+        <v>673</v>
       </c>
       <c r="U95" s="150">
-        <v>521</v>
+        <v>713</v>
       </c>
       <c r="V95" s="150">
-        <v>433</v>
+        <v>625</v>
       </c>
       <c r="W95" s="150">
-        <v>529</v>
+        <v>721</v>
       </c>
       <c r="X95" s="150">
-        <v>441</v>
+        <v>633</v>
       </c>
       <c r="Y95" s="150">
-        <v>537</v>
+        <v>729</v>
       </c>
     </row>
     <row r="96" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A96" s="247" t="s">
         <v>187</v>
       </c>
-      <c r="B96" s="133">
-        <v>1217</v>
-      </c>
-      <c r="C96" s="133">
-        <v>1125</v>
-      </c>
-      <c r="D96" s="133">
-        <v>1225</v>
-      </c>
-      <c r="E96" s="133">
-        <v>1133</v>
-      </c>
-      <c r="F96" s="133">
-        <v>1233</v>
-      </c>
-      <c r="G96" s="133">
-        <v>1141</v>
-      </c>
-      <c r="H96" s="133">
-        <v>1241</v>
-      </c>
-      <c r="I96" s="133">
-        <v>1149</v>
-      </c>
-      <c r="J96" s="133">
-        <v>1249</v>
-      </c>
-      <c r="K96" s="289" t="s">
+      <c r="B96" s="272">
+        <v>904</v>
+      </c>
+      <c r="C96" s="272">
+        <v>810</v>
+      </c>
+      <c r="D96" s="272">
+        <v>912</v>
+      </c>
+      <c r="E96" s="272">
+        <v>818</v>
+      </c>
+      <c r="F96" s="272">
+        <v>920</v>
+      </c>
+      <c r="G96" s="272">
+        <v>826</v>
+      </c>
+      <c r="H96" s="272">
+        <v>928</v>
+      </c>
+      <c r="I96" s="272">
+        <v>834</v>
+      </c>
+      <c r="J96" s="272">
+        <v>936</v>
+      </c>
+      <c r="K96" s="277" t="s">
         <v>236</v>
       </c>
-      <c r="L96" s="289"/>
-      <c r="M96" s="289"/>
-      <c r="N96" s="133">
-        <v>1157</v>
-      </c>
-      <c r="O96" s="133">
-        <v>1257</v>
-      </c>
-      <c r="P96" s="133">
-        <v>1165</v>
-      </c>
-      <c r="Q96" s="133">
-        <v>1265</v>
-      </c>
-      <c r="R96" s="133">
-        <v>1173</v>
-      </c>
-      <c r="S96" s="133">
-        <v>1273</v>
+      <c r="L96" s="277"/>
+      <c r="M96" s="277"/>
+      <c r="N96" s="272">
+        <v>842</v>
+      </c>
+      <c r="O96" s="272">
+        <v>944</v>
+      </c>
+      <c r="P96" s="272">
+        <v>850</v>
+      </c>
+      <c r="Q96" s="272">
+        <v>952</v>
+      </c>
+      <c r="R96" s="272">
+        <v>858</v>
+      </c>
+      <c r="S96" s="272">
+        <v>960</v>
       </c>
       <c r="T96" s="150">
-        <v>673</v>
+        <v>482</v>
       </c>
       <c r="U96" s="150">
-        <v>713</v>
+        <v>522</v>
       </c>
       <c r="V96" s="150">
-        <v>625</v>
+        <v>434</v>
       </c>
       <c r="W96" s="150">
-        <v>721</v>
+        <v>530</v>
       </c>
       <c r="X96" s="150">
-        <v>633</v>
+        <v>442</v>
       </c>
       <c r="Y96" s="150">
-        <v>729</v>
+        <v>538</v>
       </c>
     </row>
     <row r="97" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A97" s="247" t="s">
         <v>188</v>
       </c>
-      <c r="B97" s="133">
-        <v>904</v>
-      </c>
-      <c r="C97" s="133">
-        <v>810</v>
-      </c>
-      <c r="D97" s="133">
-        <v>912</v>
-      </c>
-      <c r="E97" s="133">
-        <v>818</v>
-      </c>
-      <c r="F97" s="133">
-        <v>920</v>
-      </c>
-      <c r="G97" s="133">
-        <v>826</v>
-      </c>
-      <c r="H97" s="133">
-        <v>928</v>
-      </c>
-      <c r="I97" s="133">
-        <v>834</v>
-      </c>
-      <c r="J97" s="133">
-        <v>936</v>
-      </c>
-      <c r="K97" s="289" t="s">
+      <c r="B97" s="272">
+        <v>1218</v>
+      </c>
+      <c r="C97" s="272">
+        <v>1126</v>
+      </c>
+      <c r="D97" s="272">
+        <v>1226</v>
+      </c>
+      <c r="E97" s="272">
+        <v>1134</v>
+      </c>
+      <c r="F97" s="272">
+        <v>1234</v>
+      </c>
+      <c r="G97" s="272">
+        <v>1142</v>
+      </c>
+      <c r="H97" s="272">
+        <v>1242</v>
+      </c>
+      <c r="I97" s="272">
+        <v>1150</v>
+      </c>
+      <c r="J97" s="272">
+        <v>1250</v>
+      </c>
+      <c r="K97" s="277" t="s">
         <v>236</v>
       </c>
-      <c r="L97" s="289"/>
-      <c r="M97" s="289"/>
-      <c r="N97" s="133">
-        <v>842</v>
-      </c>
-      <c r="O97" s="133">
-        <v>944</v>
-      </c>
-      <c r="P97" s="133">
-        <v>850</v>
-      </c>
-      <c r="Q97" s="133">
-        <v>952</v>
-      </c>
-      <c r="R97" s="133">
-        <v>858</v>
-      </c>
-      <c r="S97" s="133">
-        <v>960</v>
+      <c r="L97" s="277"/>
+      <c r="M97" s="277"/>
+      <c r="N97" s="272">
+        <v>1158</v>
+      </c>
+      <c r="O97" s="272">
+        <v>1258</v>
+      </c>
+      <c r="P97" s="272">
+        <v>1166</v>
+      </c>
+      <c r="Q97" s="272">
+        <v>1266</v>
+      </c>
+      <c r="R97" s="272">
+        <v>1174</v>
+      </c>
+      <c r="S97" s="272">
+        <v>1274</v>
       </c>
       <c r="T97" s="150">
-        <v>482</v>
+        <v>674</v>
       </c>
       <c r="U97" s="150">
-        <v>522</v>
+        <v>714</v>
       </c>
       <c r="V97" s="150">
-        <v>434</v>
+        <v>626</v>
       </c>
       <c r="W97" s="150">
-        <v>530</v>
+        <v>722</v>
       </c>
       <c r="X97" s="150">
-        <v>442</v>
+        <v>634</v>
       </c>
       <c r="Y97" s="150">
-        <v>538</v>
+        <v>730</v>
       </c>
     </row>
     <row r="98" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A98" s="247" t="s">
         <v>189</v>
       </c>
-      <c r="B98" s="133">
-        <v>1218</v>
-      </c>
-      <c r="C98" s="133">
-        <v>1126</v>
-      </c>
-      <c r="D98" s="133">
-        <v>1226</v>
-      </c>
-      <c r="E98" s="133">
-        <v>1134</v>
-      </c>
-      <c r="F98" s="133">
-        <v>1234</v>
-      </c>
-      <c r="G98" s="133">
-        <v>1142</v>
-      </c>
-      <c r="H98" s="133">
-        <v>1242</v>
-      </c>
-      <c r="I98" s="133">
-        <v>1150</v>
-      </c>
-      <c r="J98" s="133">
-        <v>1250</v>
-      </c>
-      <c r="K98" s="289" t="s">
+      <c r="B98" s="272">
+        <v>905</v>
+      </c>
+      <c r="C98" s="272">
+        <v>811</v>
+      </c>
+      <c r="D98" s="272">
+        <v>913</v>
+      </c>
+      <c r="E98" s="272">
+        <v>819</v>
+      </c>
+      <c r="F98" s="272">
+        <v>921</v>
+      </c>
+      <c r="G98" s="272">
+        <v>827</v>
+      </c>
+      <c r="H98" s="272">
+        <v>929</v>
+      </c>
+      <c r="I98" s="272">
+        <v>835</v>
+      </c>
+      <c r="J98" s="272">
+        <v>937</v>
+      </c>
+      <c r="K98" s="277" t="s">
         <v>236</v>
       </c>
-      <c r="L98" s="289"/>
-      <c r="M98" s="289"/>
-      <c r="N98" s="133">
-        <v>1158</v>
-      </c>
-      <c r="O98" s="133">
-        <v>1258</v>
-      </c>
-      <c r="P98" s="133">
-        <v>1166</v>
-      </c>
-      <c r="Q98" s="133">
-        <v>1266</v>
-      </c>
-      <c r="R98" s="133">
-        <v>1174</v>
-      </c>
-      <c r="S98" s="133">
-        <v>1274</v>
+      <c r="L98" s="277"/>
+      <c r="M98" s="277"/>
+      <c r="N98" s="272">
+        <v>843</v>
+      </c>
+      <c r="O98" s="272">
+        <v>945</v>
+      </c>
+      <c r="P98" s="272">
+        <v>851</v>
+      </c>
+      <c r="Q98" s="272">
+        <v>953</v>
+      </c>
+      <c r="R98" s="272">
+        <v>859</v>
+      </c>
+      <c r="S98" s="272">
+        <v>961</v>
       </c>
       <c r="T98" s="150">
-        <v>674</v>
+        <v>483</v>
       </c>
       <c r="U98" s="150">
-        <v>714</v>
+        <v>523</v>
       </c>
       <c r="V98" s="150">
-        <v>626</v>
+        <v>435</v>
       </c>
       <c r="W98" s="150">
-        <v>722</v>
+        <v>531</v>
       </c>
       <c r="X98" s="150">
-        <v>634</v>
+        <v>443</v>
       </c>
       <c r="Y98" s="150">
-        <v>730</v>
+        <v>539</v>
       </c>
     </row>
     <row r="99" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A99" s="247" t="s">
         <v>190</v>
       </c>
-      <c r="B99" s="133">
-        <v>905</v>
-      </c>
-      <c r="C99" s="133">
-        <v>811</v>
-      </c>
-      <c r="D99" s="133">
-        <v>913</v>
-      </c>
-      <c r="E99" s="133">
-        <v>819</v>
-      </c>
-      <c r="F99" s="133">
-        <v>921</v>
-      </c>
-      <c r="G99" s="133">
-        <v>827</v>
-      </c>
-      <c r="H99" s="133">
-        <v>929</v>
-      </c>
-      <c r="I99" s="133">
-        <v>835</v>
-      </c>
-      <c r="J99" s="133">
-        <v>937</v>
-      </c>
-      <c r="K99" s="289" t="s">
+      <c r="B99" s="272">
+        <v>1219</v>
+      </c>
+      <c r="C99" s="272">
+        <v>1127</v>
+      </c>
+      <c r="D99" s="272">
+        <v>1227</v>
+      </c>
+      <c r="E99" s="272">
+        <v>1135</v>
+      </c>
+      <c r="F99" s="272">
+        <v>1235</v>
+      </c>
+      <c r="G99" s="272">
+        <v>1143</v>
+      </c>
+      <c r="H99" s="272">
+        <v>1243</v>
+      </c>
+      <c r="I99" s="272">
+        <v>1151</v>
+      </c>
+      <c r="J99" s="272">
+        <v>1251</v>
+      </c>
+      <c r="K99" s="277" t="s">
         <v>236</v>
       </c>
-      <c r="L99" s="289"/>
-      <c r="M99" s="289"/>
-      <c r="N99" s="133">
-        <v>843</v>
-      </c>
-      <c r="O99" s="133">
-        <v>945</v>
-      </c>
-      <c r="P99" s="133">
-        <v>851</v>
-      </c>
-      <c r="Q99" s="133">
-        <v>953</v>
-      </c>
-      <c r="R99" s="133">
-        <v>859</v>
-      </c>
-      <c r="S99" s="133">
-        <v>961</v>
+      <c r="L99" s="277"/>
+      <c r="M99" s="277"/>
+      <c r="N99" s="272">
+        <v>1159</v>
+      </c>
+      <c r="O99" s="272">
+        <v>1259</v>
+      </c>
+      <c r="P99" s="272">
+        <v>1167</v>
+      </c>
+      <c r="Q99" s="272">
+        <v>1267</v>
+      </c>
+      <c r="R99" s="272">
+        <v>1175</v>
+      </c>
+      <c r="S99" s="272">
+        <v>1275</v>
       </c>
       <c r="T99" s="150">
-        <v>483</v>
+        <v>675</v>
       </c>
       <c r="U99" s="150">
-        <v>523</v>
+        <v>715</v>
       </c>
       <c r="V99" s="150">
-        <v>435</v>
+        <v>627</v>
       </c>
       <c r="W99" s="150">
-        <v>531</v>
+        <v>723</v>
       </c>
       <c r="X99" s="150">
-        <v>443</v>
+        <v>635</v>
       </c>
       <c r="Y99" s="150">
-        <v>539</v>
+        <v>731</v>
       </c>
     </row>
     <row r="100" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A100" s="247" t="s">
         <v>191</v>
       </c>
-      <c r="B100" s="133">
-        <v>1219</v>
-      </c>
-      <c r="C100" s="133">
-        <v>1127</v>
-      </c>
-      <c r="D100" s="133">
-        <v>1227</v>
-      </c>
-      <c r="E100" s="133">
-        <v>1135</v>
-      </c>
-      <c r="F100" s="133">
-        <v>1235</v>
-      </c>
-      <c r="G100" s="133">
-        <v>1143</v>
-      </c>
-      <c r="H100" s="133">
-        <v>1243</v>
-      </c>
-      <c r="I100" s="133">
-        <v>1151</v>
-      </c>
-      <c r="J100" s="133">
-        <v>1251</v>
-      </c>
-      <c r="K100" s="289" t="s">
+      <c r="B100" s="272">
+        <v>906</v>
+      </c>
+      <c r="C100" s="272">
+        <v>812</v>
+      </c>
+      <c r="D100" s="272">
+        <v>914</v>
+      </c>
+      <c r="E100" s="272">
+        <v>820</v>
+      </c>
+      <c r="F100" s="272">
+        <v>922</v>
+      </c>
+      <c r="G100" s="272">
+        <v>828</v>
+      </c>
+      <c r="H100" s="272">
+        <v>930</v>
+      </c>
+      <c r="I100" s="272">
+        <v>836</v>
+      </c>
+      <c r="J100" s="272">
+        <v>938</v>
+      </c>
+      <c r="K100" s="277" t="s">
         <v>236</v>
       </c>
-      <c r="L100" s="289"/>
-      <c r="M100" s="289"/>
-      <c r="N100" s="133">
-        <v>1159</v>
-      </c>
-      <c r="O100" s="133">
-        <v>1259</v>
-      </c>
-      <c r="P100" s="133">
-        <v>1167</v>
-      </c>
-      <c r="Q100" s="133">
-        <v>1267</v>
-      </c>
-      <c r="R100" s="133">
-        <v>1175</v>
-      </c>
-      <c r="S100" s="133">
-        <v>1275</v>
+      <c r="L100" s="277"/>
+      <c r="M100" s="277"/>
+      <c r="N100" s="272">
+        <v>844</v>
+      </c>
+      <c r="O100" s="272">
+        <v>946</v>
+      </c>
+      <c r="P100" s="272">
+        <v>852</v>
+      </c>
+      <c r="Q100" s="272">
+        <v>954</v>
+      </c>
+      <c r="R100" s="272">
+        <v>860</v>
+      </c>
+      <c r="S100" s="272">
+        <v>962</v>
       </c>
       <c r="T100" s="150">
-        <v>675</v>
+        <v>484</v>
       </c>
       <c r="U100" s="150">
-        <v>715</v>
+        <v>524</v>
       </c>
       <c r="V100" s="150">
-        <v>627</v>
+        <v>436</v>
       </c>
       <c r="W100" s="150">
-        <v>723</v>
+        <v>532</v>
       </c>
       <c r="X100" s="150">
-        <v>635</v>
+        <v>444</v>
       </c>
       <c r="Y100" s="150">
-        <v>731</v>
+        <v>540</v>
       </c>
     </row>
     <row r="101" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A101" s="247" t="s">
         <v>192</v>
       </c>
-      <c r="B101" s="133">
-        <v>906</v>
-      </c>
-      <c r="C101" s="133">
-        <v>812</v>
-      </c>
-      <c r="D101" s="133">
-        <v>914</v>
-      </c>
-      <c r="E101" s="133">
-        <v>820</v>
-      </c>
-      <c r="F101" s="133">
-        <v>922</v>
-      </c>
-      <c r="G101" s="133">
-        <v>828</v>
-      </c>
-      <c r="H101" s="133">
-        <v>930</v>
-      </c>
-      <c r="I101" s="133">
-        <v>836</v>
-      </c>
-      <c r="J101" s="133">
-        <v>938</v>
-      </c>
-      <c r="K101" s="289" t="s">
+      <c r="B101" s="272">
+        <v>1220</v>
+      </c>
+      <c r="C101" s="272">
+        <v>1128</v>
+      </c>
+      <c r="D101" s="272">
+        <v>1228</v>
+      </c>
+      <c r="E101" s="272">
+        <v>1136</v>
+      </c>
+      <c r="F101" s="272">
+        <v>1236</v>
+      </c>
+      <c r="G101" s="272">
+        <v>1144</v>
+      </c>
+      <c r="H101" s="272">
+        <v>1244</v>
+      </c>
+      <c r="I101" s="272">
+        <v>1152</v>
+      </c>
+      <c r="J101" s="272">
+        <v>1252</v>
+      </c>
+      <c r="K101" s="277" t="s">
         <v>236</v>
       </c>
-      <c r="L101" s="289"/>
-      <c r="M101" s="289"/>
-      <c r="N101" s="133">
-        <v>844</v>
-      </c>
-      <c r="O101" s="133">
-        <v>946</v>
-      </c>
-      <c r="P101" s="133">
-        <v>852</v>
-      </c>
-      <c r="Q101" s="133">
-        <v>954</v>
-      </c>
-      <c r="R101" s="133">
-        <v>860</v>
-      </c>
-      <c r="S101" s="133">
-        <v>962</v>
+      <c r="L101" s="277"/>
+      <c r="M101" s="277"/>
+      <c r="N101" s="272">
+        <v>1160</v>
+      </c>
+      <c r="O101" s="272">
+        <v>1260</v>
+      </c>
+      <c r="P101" s="272">
+        <v>1168</v>
+      </c>
+      <c r="Q101" s="272">
+        <v>1268</v>
+      </c>
+      <c r="R101" s="272">
+        <v>1176</v>
+      </c>
+      <c r="S101" s="272">
+        <v>1276</v>
       </c>
       <c r="T101" s="150">
-        <v>484</v>
+        <v>676</v>
       </c>
       <c r="U101" s="150">
-        <v>524</v>
+        <v>716</v>
       </c>
       <c r="V101" s="150">
-        <v>436</v>
+        <v>628</v>
       </c>
       <c r="W101" s="150">
-        <v>532</v>
+        <v>724</v>
       </c>
       <c r="X101" s="150">
-        <v>444</v>
+        <v>636</v>
       </c>
       <c r="Y101" s="150">
-        <v>540</v>
+        <v>732</v>
       </c>
     </row>
     <row r="102" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A102" s="247" t="s">
         <v>193</v>
       </c>
-      <c r="B102" s="133">
-        <v>1220</v>
-      </c>
-      <c r="C102" s="133">
-        <v>1128</v>
-      </c>
-      <c r="D102" s="133">
-        <v>1228</v>
-      </c>
-      <c r="E102" s="133">
-        <v>1136</v>
-      </c>
-      <c r="F102" s="133">
-        <v>1236</v>
-      </c>
-      <c r="G102" s="133">
-        <v>1144</v>
-      </c>
-      <c r="H102" s="133">
-        <v>1244</v>
-      </c>
-      <c r="I102" s="133">
-        <v>1152</v>
-      </c>
-      <c r="J102" s="133">
-        <v>1252</v>
-      </c>
-      <c r="K102" s="289" t="s">
+      <c r="B102" s="272">
+        <v>907</v>
+      </c>
+      <c r="C102" s="272">
+        <v>813</v>
+      </c>
+      <c r="D102" s="272">
+        <v>915</v>
+      </c>
+      <c r="E102" s="272">
+        <v>821</v>
+      </c>
+      <c r="F102" s="272">
+        <v>923</v>
+      </c>
+      <c r="G102" s="272">
+        <v>829</v>
+      </c>
+      <c r="H102" s="272">
+        <v>931</v>
+      </c>
+      <c r="I102" s="272">
+        <v>837</v>
+      </c>
+      <c r="J102" s="272">
+        <v>939</v>
+      </c>
+      <c r="K102" s="277" t="s">
         <v>236</v>
       </c>
-      <c r="L102" s="289"/>
-      <c r="M102" s="289"/>
-      <c r="N102" s="133">
-        <v>1160</v>
-      </c>
-      <c r="O102" s="133">
-        <v>1260</v>
-      </c>
-      <c r="P102" s="133">
-        <v>1168</v>
-      </c>
-      <c r="Q102" s="133">
-        <v>1268</v>
-      </c>
-      <c r="R102" s="133">
-        <v>1176</v>
-      </c>
-      <c r="S102" s="133">
-        <v>1276</v>
+      <c r="L102" s="277"/>
+      <c r="M102" s="277"/>
+      <c r="N102" s="272">
+        <v>845</v>
+      </c>
+      <c r="O102" s="272">
+        <v>947</v>
+      </c>
+      <c r="P102" s="272">
+        <v>853</v>
+      </c>
+      <c r="Q102" s="272">
+        <v>955</v>
+      </c>
+      <c r="R102" s="272">
+        <v>867</v>
+      </c>
+      <c r="S102" s="272">
+        <v>963</v>
       </c>
       <c r="T102" s="150">
-        <v>676</v>
+        <v>485</v>
       </c>
       <c r="U102" s="150">
-        <v>716</v>
+        <v>525</v>
       </c>
       <c r="V102" s="150">
-        <v>628</v>
+        <v>437</v>
       </c>
       <c r="W102" s="150">
-        <v>724</v>
+        <v>533</v>
       </c>
       <c r="X102" s="150">
-        <v>636</v>
+        <v>445</v>
       </c>
       <c r="Y102" s="150">
-        <v>732</v>
+        <v>541</v>
       </c>
     </row>
     <row r="103" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A103" s="247" t="s">
         <v>194</v>
       </c>
-      <c r="B103" s="133">
-        <v>907</v>
-      </c>
-      <c r="C103" s="133">
-        <v>813</v>
-      </c>
-      <c r="D103" s="133">
-        <v>915</v>
-      </c>
-      <c r="E103" s="133">
-        <v>821</v>
-      </c>
-      <c r="F103" s="133">
-        <v>923</v>
-      </c>
-      <c r="G103" s="133">
-        <v>829</v>
-      </c>
-      <c r="H103" s="133">
-        <v>931</v>
-      </c>
-      <c r="I103" s="133">
-        <v>837</v>
-      </c>
-      <c r="J103" s="133">
-        <v>939</v>
-      </c>
-      <c r="K103" s="289" t="s">
+      <c r="B103" s="272">
+        <v>1221</v>
+      </c>
+      <c r="C103" s="272">
+        <v>1129</v>
+      </c>
+      <c r="D103" s="272">
+        <v>1229</v>
+      </c>
+      <c r="E103" s="272">
+        <v>1137</v>
+      </c>
+      <c r="F103" s="272">
+        <v>1237</v>
+      </c>
+      <c r="G103" s="272">
+        <v>1145</v>
+      </c>
+      <c r="H103" s="272">
+        <v>1245</v>
+      </c>
+      <c r="I103" s="272">
+        <v>1153</v>
+      </c>
+      <c r="J103" s="272">
+        <v>1253</v>
+      </c>
+      <c r="K103" s="277" t="s">
         <v>236</v>
       </c>
-      <c r="L103" s="289"/>
-      <c r="M103" s="289"/>
-      <c r="N103" s="133">
-        <v>845</v>
-      </c>
-      <c r="O103" s="133">
-        <v>947</v>
-      </c>
-      <c r="P103" s="133">
-        <v>853</v>
-      </c>
-      <c r="Q103" s="133">
-        <v>955</v>
-      </c>
-      <c r="R103" s="133">
-        <v>867</v>
-      </c>
-      <c r="S103" s="133">
-        <v>963</v>
+      <c r="L103" s="277"/>
+      <c r="M103" s="277"/>
+      <c r="N103" s="272">
+        <v>1161</v>
+      </c>
+      <c r="O103" s="272">
+        <v>1261</v>
+      </c>
+      <c r="P103" s="272">
+        <v>1169</v>
+      </c>
+      <c r="Q103" s="272">
+        <v>1269</v>
+      </c>
+      <c r="R103" s="272">
+        <v>1177</v>
+      </c>
+      <c r="S103" s="272">
+        <v>1277</v>
       </c>
       <c r="T103" s="150">
-        <v>485</v>
+        <v>677</v>
       </c>
       <c r="U103" s="150">
-        <v>525</v>
+        <v>717</v>
       </c>
       <c r="V103" s="150">
-        <v>437</v>
+        <v>629</v>
       </c>
       <c r="W103" s="150">
-        <v>533</v>
+        <v>725</v>
       </c>
       <c r="X103" s="150">
-        <v>445</v>
+        <v>637</v>
       </c>
       <c r="Y103" s="150">
-        <v>541</v>
+        <v>733</v>
       </c>
     </row>
     <row r="104" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A104" s="247" t="s">
         <v>195</v>
       </c>
-      <c r="B104" s="133">
-        <v>1221</v>
-      </c>
-      <c r="C104" s="133">
-        <v>1129</v>
-      </c>
-      <c r="D104" s="133">
-        <v>1229</v>
-      </c>
-      <c r="E104" s="133">
-        <v>1137</v>
-      </c>
-      <c r="F104" s="133">
-        <v>1237</v>
-      </c>
-      <c r="G104" s="133">
-        <v>1145</v>
-      </c>
-      <c r="H104" s="133">
-        <v>1245</v>
-      </c>
-      <c r="I104" s="133">
-        <v>1153</v>
-      </c>
-      <c r="J104" s="133">
-        <v>1253</v>
-      </c>
-      <c r="K104" s="289" t="s">
+      <c r="B104" s="272">
+        <v>908</v>
+      </c>
+      <c r="C104" s="272">
+        <v>814</v>
+      </c>
+      <c r="D104" s="272">
+        <v>916</v>
+      </c>
+      <c r="E104" s="272">
+        <v>822</v>
+      </c>
+      <c r="F104" s="272">
+        <v>924</v>
+      </c>
+      <c r="G104" s="272">
+        <v>830</v>
+      </c>
+      <c r="H104" s="272">
+        <v>932</v>
+      </c>
+      <c r="I104" s="272">
+        <v>838</v>
+      </c>
+      <c r="J104" s="272">
+        <v>940</v>
+      </c>
+      <c r="K104" s="277" t="s">
         <v>236</v>
       </c>
-      <c r="L104" s="289"/>
-      <c r="M104" s="289"/>
-      <c r="N104" s="133">
-        <v>1161</v>
-      </c>
-      <c r="O104" s="133">
-        <v>1261</v>
-      </c>
-      <c r="P104" s="133">
-        <v>1169</v>
-      </c>
-      <c r="Q104" s="133">
-        <v>1269</v>
-      </c>
-      <c r="R104" s="133">
-        <v>1177</v>
-      </c>
-      <c r="S104" s="133">
-        <v>1277</v>
+      <c r="L104" s="277"/>
+      <c r="M104" s="277"/>
+      <c r="N104" s="272">
+        <v>846</v>
+      </c>
+      <c r="O104" s="272">
+        <v>948</v>
+      </c>
+      <c r="P104" s="272">
+        <v>854</v>
+      </c>
+      <c r="Q104" s="272">
+        <v>956</v>
+      </c>
+      <c r="R104" s="272">
+        <v>868</v>
+      </c>
+      <c r="S104" s="272">
+        <v>964</v>
       </c>
       <c r="T104" s="150">
-        <v>677</v>
+        <v>486</v>
       </c>
       <c r="U104" s="150">
-        <v>717</v>
+        <v>526</v>
       </c>
       <c r="V104" s="150">
-        <v>629</v>
+        <v>438</v>
       </c>
       <c r="W104" s="150">
-        <v>725</v>
+        <v>534</v>
       </c>
       <c r="X104" s="150">
-        <v>637</v>
+        <v>446</v>
       </c>
       <c r="Y104" s="150">
-        <v>733</v>
+        <v>542</v>
       </c>
     </row>
     <row r="105" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A105" s="247" t="s">
         <v>196</v>
       </c>
-      <c r="B105" s="133">
-        <v>908</v>
-      </c>
-      <c r="C105" s="133">
-        <v>814</v>
-      </c>
-      <c r="D105" s="133">
-        <v>916</v>
-      </c>
-      <c r="E105" s="133">
-        <v>822</v>
-      </c>
-      <c r="F105" s="133">
-        <v>924</v>
-      </c>
-      <c r="G105" s="133">
-        <v>830</v>
-      </c>
-      <c r="H105" s="133">
-        <v>932</v>
-      </c>
-      <c r="I105" s="133">
-        <v>838</v>
-      </c>
-      <c r="J105" s="133">
-        <v>940</v>
-      </c>
-      <c r="K105" s="289" t="s">
+      <c r="B105" s="272">
+        <v>1222</v>
+      </c>
+      <c r="C105" s="272">
+        <v>1130</v>
+      </c>
+      <c r="D105" s="272">
+        <v>1230</v>
+      </c>
+      <c r="E105" s="272">
+        <v>1138</v>
+      </c>
+      <c r="F105" s="272">
+        <v>1238</v>
+      </c>
+      <c r="G105" s="272">
+        <v>1146</v>
+      </c>
+      <c r="H105" s="272">
+        <v>1246</v>
+      </c>
+      <c r="I105" s="272">
+        <v>1154</v>
+      </c>
+      <c r="J105" s="272">
+        <v>1254</v>
+      </c>
+      <c r="K105" s="277" t="s">
         <v>236</v>
       </c>
-      <c r="L105" s="289"/>
-      <c r="M105" s="289"/>
-      <c r="N105" s="133">
-        <v>846</v>
-      </c>
-      <c r="O105" s="133">
-        <v>948</v>
-      </c>
-      <c r="P105" s="133">
-        <v>854</v>
-      </c>
-      <c r="Q105" s="133">
-        <v>956</v>
-      </c>
-      <c r="R105" s="133">
-        <v>868</v>
-      </c>
-      <c r="S105" s="133">
-        <v>964</v>
+      <c r="L105" s="277"/>
+      <c r="M105" s="277"/>
+      <c r="N105" s="272">
+        <v>1162</v>
+      </c>
+      <c r="O105" s="272">
+        <v>1262</v>
+      </c>
+      <c r="P105" s="272">
+        <v>1170</v>
+      </c>
+      <c r="Q105" s="272">
+        <v>1270</v>
+      </c>
+      <c r="R105" s="272">
+        <v>1178</v>
+      </c>
+      <c r="S105" s="272">
+        <v>1278</v>
       </c>
       <c r="T105" s="150">
-        <v>486</v>
+        <v>678</v>
       </c>
       <c r="U105" s="150">
-        <v>526</v>
+        <v>718</v>
       </c>
       <c r="V105" s="150">
-        <v>438</v>
+        <v>630</v>
       </c>
       <c r="W105" s="150">
-        <v>534</v>
+        <v>726</v>
       </c>
       <c r="X105" s="150">
-        <v>446</v>
+        <v>638</v>
       </c>
       <c r="Y105" s="150">
-        <v>542</v>
+        <v>734</v>
       </c>
     </row>
     <row r="106" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A106" s="247" t="s">
         <v>197</v>
       </c>
-      <c r="B106" s="133">
-        <v>1222</v>
-      </c>
-      <c r="C106" s="133">
-        <v>1130</v>
-      </c>
-      <c r="D106" s="133">
-        <v>1230</v>
-      </c>
-      <c r="E106" s="133">
-        <v>1138</v>
-      </c>
-      <c r="F106" s="133">
-        <v>1238</v>
-      </c>
-      <c r="G106" s="133">
-        <v>1146</v>
-      </c>
-      <c r="H106" s="133">
-        <v>1246</v>
-      </c>
-      <c r="I106" s="133">
-        <v>1154</v>
-      </c>
-      <c r="J106" s="133">
-        <v>1254</v>
-      </c>
-      <c r="K106" s="289" t="s">
+      <c r="B106" s="272">
+        <v>909</v>
+      </c>
+      <c r="C106" s="272">
+        <v>815</v>
+      </c>
+      <c r="D106" s="272">
+        <v>917</v>
+      </c>
+      <c r="E106" s="272">
+        <v>823</v>
+      </c>
+      <c r="F106" s="272">
+        <v>925</v>
+      </c>
+      <c r="G106" s="272">
+        <v>831</v>
+      </c>
+      <c r="H106" s="272">
+        <v>933</v>
+      </c>
+      <c r="I106" s="272">
+        <v>839</v>
+      </c>
+      <c r="J106" s="272">
+        <v>941</v>
+      </c>
+      <c r="K106" s="277" t="s">
         <v>236</v>
       </c>
-      <c r="L106" s="289"/>
-      <c r="M106" s="289"/>
-      <c r="N106" s="133">
-        <v>1162</v>
-      </c>
-      <c r="O106" s="133">
-        <v>1262</v>
-      </c>
-      <c r="P106" s="133">
-        <v>1170</v>
-      </c>
-      <c r="Q106" s="133">
-        <v>1270</v>
-      </c>
-      <c r="R106" s="133">
-        <v>1178</v>
-      </c>
-      <c r="S106" s="133">
-        <v>1278</v>
+      <c r="L106" s="277"/>
+      <c r="M106" s="277"/>
+      <c r="N106" s="272">
+        <v>847</v>
+      </c>
+      <c r="O106" s="272">
+        <v>949</v>
+      </c>
+      <c r="P106" s="272">
+        <v>855</v>
+      </c>
+      <c r="Q106" s="272">
+        <v>957</v>
+      </c>
+      <c r="R106" s="272">
+        <v>869</v>
+      </c>
+      <c r="S106" s="272">
+        <v>965</v>
       </c>
       <c r="T106" s="150">
-        <v>678</v>
+        <v>487</v>
       </c>
       <c r="U106" s="150">
-        <v>718</v>
+        <v>527</v>
       </c>
       <c r="V106" s="150">
-        <v>630</v>
+        <v>439</v>
       </c>
       <c r="W106" s="150">
-        <v>726</v>
+        <v>535</v>
       </c>
       <c r="X106" s="150">
-        <v>638</v>
+        <v>447</v>
       </c>
       <c r="Y106" s="150">
-        <v>734</v>
+        <v>543</v>
       </c>
     </row>
     <row r="107" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A107" s="247" t="s">
         <v>198</v>
       </c>
-      <c r="B107" s="133">
-        <v>909</v>
-      </c>
-      <c r="C107" s="133">
-        <v>815</v>
-      </c>
-      <c r="D107" s="133">
-        <v>917</v>
-      </c>
-      <c r="E107" s="133">
-        <v>823</v>
-      </c>
-      <c r="F107" s="133">
-        <v>925</v>
-      </c>
-      <c r="G107" s="133">
-        <v>831</v>
-      </c>
-      <c r="H107" s="133">
-        <v>933</v>
-      </c>
-      <c r="I107" s="133">
-        <v>839</v>
-      </c>
-      <c r="J107" s="133">
-        <v>941</v>
-      </c>
-      <c r="K107" s="289" t="s">
+      <c r="B107" s="272">
+        <v>1223</v>
+      </c>
+      <c r="C107" s="272">
+        <v>1131</v>
+      </c>
+      <c r="D107" s="272">
+        <v>1231</v>
+      </c>
+      <c r="E107" s="272">
+        <v>1139</v>
+      </c>
+      <c r="F107" s="272">
+        <v>1239</v>
+      </c>
+      <c r="G107" s="272">
+        <v>1147</v>
+      </c>
+      <c r="H107" s="272">
+        <v>1247</v>
+      </c>
+      <c r="I107" s="272">
+        <v>1155</v>
+      </c>
+      <c r="J107" s="272">
+        <v>1255</v>
+      </c>
+      <c r="K107" s="277" t="s">
         <v>236</v>
       </c>
-      <c r="L107" s="289"/>
-      <c r="M107" s="289"/>
-      <c r="N107" s="133">
-        <v>847</v>
-      </c>
-      <c r="O107" s="133">
-        <v>949</v>
-      </c>
-      <c r="P107" s="133">
-        <v>855</v>
-      </c>
-      <c r="Q107" s="133">
-        <v>957</v>
-      </c>
-      <c r="R107" s="133">
-        <v>869</v>
-      </c>
-      <c r="S107" s="133">
-        <v>965</v>
+      <c r="L107" s="277"/>
+      <c r="M107" s="277"/>
+      <c r="N107" s="272">
+        <v>1163</v>
+      </c>
+      <c r="O107" s="272">
+        <v>1263</v>
+      </c>
+      <c r="P107" s="272">
+        <v>1171</v>
+      </c>
+      <c r="Q107" s="272">
+        <v>1271</v>
+      </c>
+      <c r="R107" s="272">
+        <v>1179</v>
+      </c>
+      <c r="S107" s="272">
+        <v>1279</v>
       </c>
       <c r="T107" s="150">
-        <v>487</v>
+        <v>679</v>
       </c>
       <c r="U107" s="150">
-        <v>527</v>
+        <v>719</v>
       </c>
       <c r="V107" s="150">
-        <v>439</v>
+        <v>631</v>
       </c>
       <c r="W107" s="150">
-        <v>535</v>
+        <v>727</v>
       </c>
       <c r="X107" s="150">
-        <v>447</v>
+        <v>639</v>
       </c>
       <c r="Y107" s="150">
-        <v>543</v>
+        <v>735</v>
       </c>
     </row>
     <row r="108" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A108" s="247" t="s">
         <v>199</v>
       </c>
-      <c r="B108" s="133">
-        <v>1223</v>
-      </c>
-      <c r="C108" s="133">
-        <v>1131</v>
-      </c>
-      <c r="D108" s="133">
-        <v>1231</v>
-      </c>
-      <c r="E108" s="133">
-        <v>1139</v>
-      </c>
-      <c r="F108" s="133">
-        <v>1239</v>
-      </c>
-      <c r="G108" s="133">
-        <v>1147</v>
-      </c>
-      <c r="H108" s="133">
-        <v>1247</v>
-      </c>
-      <c r="I108" s="133">
-        <v>1155</v>
-      </c>
-      <c r="J108" s="133">
-        <v>1255</v>
-      </c>
-      <c r="K108" s="289" t="s">
+      <c r="B108" s="272">
+        <v>910</v>
+      </c>
+      <c r="C108" s="272">
+        <v>816</v>
+      </c>
+      <c r="D108" s="272">
+        <v>918</v>
+      </c>
+      <c r="E108" s="272">
+        <v>824</v>
+      </c>
+      <c r="F108" s="272">
+        <v>926</v>
+      </c>
+      <c r="G108" s="272">
+        <v>832</v>
+      </c>
+      <c r="H108" s="272">
+        <v>934</v>
+      </c>
+      <c r="I108" s="272">
+        <v>840</v>
+      </c>
+      <c r="J108" s="272">
+        <v>942</v>
+      </c>
+      <c r="K108" s="277" t="s">
         <v>236</v>
       </c>
-      <c r="L108" s="289"/>
-      <c r="M108" s="289"/>
-      <c r="N108" s="133">
-        <v>1163</v>
-      </c>
-      <c r="O108" s="133">
-        <v>1263</v>
-      </c>
-      <c r="P108" s="133">
-        <v>1171</v>
-      </c>
-      <c r="Q108" s="133">
-        <v>1271</v>
-      </c>
-      <c r="R108" s="133">
-        <v>1179</v>
-      </c>
-      <c r="S108" s="133">
-        <v>1279</v>
+      <c r="L108" s="277"/>
+      <c r="M108" s="277"/>
+      <c r="N108" s="272">
+        <v>848</v>
+      </c>
+      <c r="O108" s="272">
+        <v>950</v>
+      </c>
+      <c r="P108" s="272">
+        <v>856</v>
+      </c>
+      <c r="Q108" s="272">
+        <v>958</v>
+      </c>
+      <c r="R108" s="272">
+        <v>870</v>
+      </c>
+      <c r="S108" s="272">
+        <v>966</v>
       </c>
       <c r="T108" s="150">
-        <v>679</v>
+        <v>488</v>
       </c>
       <c r="U108" s="150">
-        <v>719</v>
+        <v>528</v>
       </c>
       <c r="V108" s="150">
-        <v>631</v>
+        <v>440</v>
       </c>
       <c r="W108" s="150">
-        <v>727</v>
+        <v>536</v>
       </c>
       <c r="X108" s="150">
-        <v>639</v>
+        <v>448</v>
       </c>
       <c r="Y108" s="150">
-        <v>735</v>
+        <v>544</v>
       </c>
     </row>
     <row r="109" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A109" s="252" t="s">
         <v>200</v>
       </c>
-      <c r="B109" s="133">
-        <v>910</v>
-      </c>
-      <c r="C109" s="133">
-        <v>816</v>
-      </c>
-      <c r="D109" s="133">
-        <v>918</v>
-      </c>
-      <c r="E109" s="133">
-        <v>824</v>
-      </c>
-      <c r="F109" s="133">
-        <v>926</v>
-      </c>
-      <c r="G109" s="133">
-        <v>832</v>
-      </c>
-      <c r="H109" s="133">
-        <v>934</v>
-      </c>
-      <c r="I109" s="133">
-        <v>840</v>
-      </c>
-      <c r="J109" s="133">
-        <v>942</v>
-      </c>
-      <c r="K109" s="289" t="s">
+      <c r="B109" s="272">
+        <v>1224</v>
+      </c>
+      <c r="C109" s="272">
+        <v>1132</v>
+      </c>
+      <c r="D109" s="272">
+        <v>1232</v>
+      </c>
+      <c r="E109" s="272">
+        <v>1140</v>
+      </c>
+      <c r="F109" s="272">
+        <v>1240</v>
+      </c>
+      <c r="G109" s="272">
+        <v>1148</v>
+      </c>
+      <c r="H109" s="272">
+        <v>1248</v>
+      </c>
+      <c r="I109" s="272">
+        <v>1156</v>
+      </c>
+      <c r="J109" s="272">
+        <v>1256</v>
+      </c>
+      <c r="K109" s="277" t="s">
         <v>235</v>
       </c>
-      <c r="L109" s="289"/>
-      <c r="M109" s="289"/>
-      <c r="N109" s="133">
-        <v>848</v>
-      </c>
-      <c r="O109" s="133">
-        <v>950</v>
-      </c>
-      <c r="P109" s="133">
-        <v>856</v>
-      </c>
-      <c r="Q109" s="133">
-        <v>958</v>
-      </c>
-      <c r="R109" s="133">
-        <v>870</v>
-      </c>
-      <c r="S109" s="133">
-        <v>966</v>
+      <c r="L109" s="277"/>
+      <c r="M109" s="277"/>
+      <c r="N109" s="272">
+        <v>1164</v>
+      </c>
+      <c r="O109" s="272">
+        <v>1264</v>
+      </c>
+      <c r="P109" s="272">
+        <v>1172</v>
+      </c>
+      <c r="Q109" s="272">
+        <v>1272</v>
+      </c>
+      <c r="R109" s="272">
+        <v>1180</v>
+      </c>
+      <c r="S109" s="272">
+        <v>1280</v>
       </c>
       <c r="T109" s="150">
-        <v>488</v>
+        <v>680</v>
       </c>
       <c r="U109" s="150">
-        <v>528</v>
+        <v>720</v>
       </c>
       <c r="V109" s="150">
-        <v>440</v>
+        <v>632</v>
       </c>
       <c r="W109" s="150">
-        <v>536</v>
+        <v>728</v>
       </c>
       <c r="X109" s="150">
-        <v>448</v>
+        <v>640</v>
       </c>
       <c r="Y109" s="150">
-        <v>544</v>
+        <v>736</v>
       </c>
     </row>
     <row r="110" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
         <v>234</v>
       </c>
-      <c r="K110" s="290" t="s">
+      <c r="K110" s="278" t="s">
         <v>243</v>
       </c>
-      <c r="L110" s="290"/>
-      <c r="M110" s="290"/>
+      <c r="L110" s="278"/>
+      <c r="M110" s="278"/>
       <c r="N110" t="s">
         <v>242</v>
       </c>
@@ -7949,6 +7950,26 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="J66:J71"/>
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="M2:O3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="R66:S66"/>
+    <mergeCell ref="T66:U66"/>
+    <mergeCell ref="X67:X71"/>
+    <mergeCell ref="W94:Y94"/>
+    <mergeCell ref="T94:V94"/>
+    <mergeCell ref="N94:S94"/>
+    <mergeCell ref="K96:M96"/>
+    <mergeCell ref="K97:M97"/>
+    <mergeCell ref="K98:M98"/>
+    <mergeCell ref="K99:M99"/>
+    <mergeCell ref="P66:Q66"/>
     <mergeCell ref="K106:M106"/>
     <mergeCell ref="K107:M107"/>
     <mergeCell ref="K110:M110"/>
@@ -7965,26 +7986,6 @@
     <mergeCell ref="K109:M109"/>
     <mergeCell ref="K108:M108"/>
     <mergeCell ref="K95:M95"/>
-    <mergeCell ref="K96:M96"/>
-    <mergeCell ref="K97:M97"/>
-    <mergeCell ref="K98:M98"/>
-    <mergeCell ref="K99:M99"/>
-    <mergeCell ref="P66:Q66"/>
-    <mergeCell ref="R66:S66"/>
-    <mergeCell ref="T66:U66"/>
-    <mergeCell ref="X67:X71"/>
-    <mergeCell ref="W94:Y94"/>
-    <mergeCell ref="T94:V94"/>
-    <mergeCell ref="N94:S94"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="J66:J71"/>
-    <mergeCell ref="B1:M1"/>
-    <mergeCell ref="M2:O3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K7:L7"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8150,20 +8151,20 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="272" t="s">
+      <c r="B1" s="273" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="273"/>
-      <c r="D1" s="273"/>
-      <c r="E1" s="273"/>
-      <c r="F1" s="273"/>
-      <c r="G1" s="273"/>
-      <c r="H1" s="273"/>
-      <c r="I1" s="273"/>
-      <c r="J1" s="273"/>
-      <c r="K1" s="273"/>
-      <c r="L1" s="273"/>
-      <c r="M1" s="274"/>
+      <c r="C1" s="274"/>
+      <c r="D1" s="274"/>
+      <c r="E1" s="274"/>
+      <c r="F1" s="274"/>
+      <c r="G1" s="274"/>
+      <c r="H1" s="274"/>
+      <c r="I1" s="274"/>
+      <c r="J1" s="274"/>
+      <c r="K1" s="274"/>
+      <c r="L1" s="274"/>
+      <c r="M1" s="275"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
     </row>
@@ -8667,10 +8668,10 @@
       <c r="E17" s="29">
         <v>1</v>
       </c>
-      <c r="G17" s="275" t="s">
+      <c r="G17" s="276" t="s">
         <v>75</v>
       </c>
-      <c r="H17" s="275"/>
+      <c r="H17" s="276"/>
       <c r="I17" s="21" t="s">
         <v>76</v>
       </c>

</xml_diff>

<commit_message>
finished analysis of screen performed on 99-20-16, compelte with markdown file which will be added to lab notebook
</commit_message>
<xml_diff>
--- a/Kamarck Ecell Transfections 2-16.xlsx
+++ b/Kamarck Ecell Transfections 2-16.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/storage/mainland/Projects/TAARs/E cell Optimization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/mainland-1/Projects/TAARs/E cell Optimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1650,7 +1650,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="294">
+  <cellXfs count="296">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -2024,16 +2024,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2072,6 +2062,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -4182,8 +4190,8 @@
   </sheetPr>
   <dimension ref="A1:Y132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="L90" sqref="L90"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="S123" sqref="S123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4192,20 +4200,20 @@
       <c r="A1" s="134" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="285" t="s">
+      <c r="B1" s="281" t="s">
         <v>232</v>
       </c>
-      <c r="C1" s="286"/>
-      <c r="D1" s="286"/>
-      <c r="E1" s="286"/>
-      <c r="F1" s="286"/>
-      <c r="G1" s="286"/>
-      <c r="H1" s="286"/>
-      <c r="I1" s="286"/>
-      <c r="J1" s="286"/>
-      <c r="K1" s="286"/>
-      <c r="L1" s="286"/>
-      <c r="M1" s="287"/>
+      <c r="C1" s="282"/>
+      <c r="D1" s="282"/>
+      <c r="E1" s="282"/>
+      <c r="F1" s="282"/>
+      <c r="G1" s="282"/>
+      <c r="H1" s="282"/>
+      <c r="I1" s="282"/>
+      <c r="J1" s="282"/>
+      <c r="K1" s="282"/>
+      <c r="L1" s="282"/>
+      <c r="M1" s="283"/>
     </row>
     <row r="2" spans="1:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="135" t="s">
@@ -4228,9 +4236,9 @@
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
-      <c r="M2" s="288"/>
-      <c r="N2" s="288"/>
-      <c r="O2" s="288"/>
+      <c r="M2" s="284"/>
+      <c r="N2" s="284"/>
+      <c r="O2" s="284"/>
     </row>
     <row r="3" spans="1:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="141" t="s">
@@ -4245,16 +4253,16 @@
       <c r="G3" s="256">
         <v>1</v>
       </c>
-      <c r="H3" s="289" t="s">
+      <c r="H3" s="285" t="s">
         <v>91</v>
       </c>
       <c r="I3" s="274"/>
       <c r="J3" s="274"/>
       <c r="K3" s="275"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="288"/>
-      <c r="N3" s="288"/>
-      <c r="O3" s="288"/>
+      <c r="M3" s="284"/>
+      <c r="N3" s="284"/>
+      <c r="O3" s="284"/>
     </row>
     <row r="4" spans="1:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="143" t="s">
@@ -4333,11 +4341,11 @@
         <f>(G5+0.2*G5)*1.11111111111111</f>
         <v>33.3333333333333</v>
       </c>
-      <c r="H6" s="290" t="s">
+      <c r="H6" s="286" t="s">
         <v>93</v>
       </c>
-      <c r="I6" s="291"/>
-      <c r="J6" s="292"/>
+      <c r="I6" s="287"/>
+      <c r="J6" s="288"/>
       <c r="K6" s="258"/>
       <c r="L6" s="3"/>
       <c r="M6" s="156" t="s">
@@ -4383,10 +4391,10 @@
       <c r="J7" s="133" t="s">
         <v>99</v>
       </c>
-      <c r="K7" s="293" t="s">
+      <c r="K7" s="289" t="s">
         <v>27</v>
       </c>
-      <c r="L7" s="293"/>
+      <c r="L7" s="289"/>
       <c r="M7" s="140" t="s">
         <v>100</v>
       </c>
@@ -6069,25 +6077,25 @@
       <c r="A66" s="247" t="s">
         <v>177</v>
       </c>
-      <c r="B66" s="281" t="s">
+      <c r="B66" s="277" t="s">
         <v>178</v>
       </c>
-      <c r="C66" s="281"/>
-      <c r="D66" s="282" t="s">
+      <c r="C66" s="277"/>
+      <c r="D66" s="278" t="s">
         <v>179</v>
       </c>
-      <c r="E66" s="282"/>
-      <c r="F66" s="283" t="s">
+      <c r="E66" s="278"/>
+      <c r="F66" s="279" t="s">
         <v>180</v>
       </c>
-      <c r="G66" s="283"/>
+      <c r="G66" s="279"/>
       <c r="H66" s="248" t="s">
         <v>181</v>
       </c>
       <c r="I66" s="249" t="s">
         <v>182</v>
       </c>
-      <c r="J66" s="284" t="s">
+      <c r="J66" s="280" t="s">
         <v>183</v>
       </c>
       <c r="K66" s="49"/>
@@ -6097,18 +6105,18 @@
       <c r="O66" s="247" t="s">
         <v>177</v>
       </c>
-      <c r="P66" s="281" t="s">
+      <c r="P66" s="277" t="s">
         <v>178</v>
       </c>
-      <c r="Q66" s="281"/>
-      <c r="R66" s="282" t="s">
+      <c r="Q66" s="277"/>
+      <c r="R66" s="278" t="s">
         <v>179</v>
       </c>
-      <c r="S66" s="282"/>
-      <c r="T66" s="283" t="s">
+      <c r="S66" s="278"/>
+      <c r="T66" s="279" t="s">
         <v>184</v>
       </c>
-      <c r="U66" s="283"/>
+      <c r="U66" s="279"/>
       <c r="V66" s="248" t="s">
         <v>181</v>
       </c>
@@ -6129,7 +6137,7 @@
       <c r="G67" s="250"/>
       <c r="H67" s="250"/>
       <c r="I67" s="250"/>
-      <c r="J67" s="284"/>
+      <c r="J67" s="280"/>
       <c r="K67" s="11"/>
       <c r="L67" s="11"/>
       <c r="M67" s="11"/>
@@ -6145,7 +6153,7 @@
       <c r="U67" s="250"/>
       <c r="V67" s="250"/>
       <c r="W67" s="250"/>
-      <c r="X67" s="284" t="s">
+      <c r="X67" s="280" t="s">
         <v>186</v>
       </c>
     </row>
@@ -6161,7 +6169,7 @@
       <c r="G68" s="250"/>
       <c r="H68" s="250"/>
       <c r="I68" s="251"/>
-      <c r="J68" s="284"/>
+      <c r="J68" s="280"/>
       <c r="K68" s="11"/>
       <c r="L68" s="11"/>
       <c r="M68" s="11"/>
@@ -6177,7 +6185,7 @@
       <c r="U68" s="250"/>
       <c r="V68" s="250"/>
       <c r="W68" s="251"/>
-      <c r="X68" s="284"/>
+      <c r="X68" s="280"/>
     </row>
     <row r="69" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A69" s="247" t="s">
@@ -6191,7 +6199,7 @@
       <c r="G69" s="250"/>
       <c r="H69" s="250"/>
       <c r="I69" s="251"/>
-      <c r="J69" s="284"/>
+      <c r="J69" s="280"/>
       <c r="K69" s="11"/>
       <c r="L69" s="11"/>
       <c r="M69" s="11"/>
@@ -6207,7 +6215,7 @@
       <c r="U69" s="250"/>
       <c r="V69" s="250"/>
       <c r="W69" s="251"/>
-      <c r="X69" s="284"/>
+      <c r="X69" s="280"/>
     </row>
     <row r="70" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A70" s="247" t="s">
@@ -6221,7 +6229,7 @@
       <c r="G70" s="250"/>
       <c r="H70" s="250"/>
       <c r="I70" s="251"/>
-      <c r="J70" s="284"/>
+      <c r="J70" s="280"/>
       <c r="K70" s="11"/>
       <c r="L70" s="11"/>
       <c r="M70" s="11"/>
@@ -6237,7 +6245,7 @@
       <c r="U70" s="250"/>
       <c r="V70" s="250"/>
       <c r="W70" s="251"/>
-      <c r="X70" s="284"/>
+      <c r="X70" s="280"/>
     </row>
     <row r="71" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A71" s="247" t="s">
@@ -6251,7 +6259,7 @@
       <c r="G71" s="250"/>
       <c r="H71" s="250"/>
       <c r="I71" s="251"/>
-      <c r="J71" s="284"/>
+      <c r="J71" s="280"/>
       <c r="K71" s="11"/>
       <c r="L71" s="11"/>
       <c r="M71" s="11"/>
@@ -6267,7 +6275,7 @@
       <c r="U71" s="250"/>
       <c r="V71" s="250"/>
       <c r="W71" s="251"/>
-      <c r="X71" s="284"/>
+      <c r="X71" s="280"/>
     </row>
     <row r="72" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A72" s="247" t="s">
@@ -6659,40 +6667,40 @@
       <c r="A94" s="247" t="s">
         <v>177</v>
       </c>
-      <c r="B94" s="279" t="s">
+      <c r="B94" s="292" t="s">
         <v>178</v>
       </c>
-      <c r="C94" s="279"/>
-      <c r="D94" s="279"/>
-      <c r="E94" s="279"/>
-      <c r="F94" s="279"/>
-      <c r="G94" s="279"/>
-      <c r="H94" s="279" t="s">
+      <c r="C94" s="292"/>
+      <c r="D94" s="292"/>
+      <c r="E94" s="292"/>
+      <c r="F94" s="292"/>
+      <c r="G94" s="292"/>
+      <c r="H94" s="292" t="s">
         <v>179</v>
       </c>
-      <c r="I94" s="279"/>
-      <c r="J94" s="279"/>
-      <c r="K94" s="279"/>
-      <c r="L94" s="279"/>
-      <c r="M94" s="279"/>
-      <c r="N94" s="277" t="s">
+      <c r="I94" s="292"/>
+      <c r="J94" s="292"/>
+      <c r="K94" s="292"/>
+      <c r="L94" s="292"/>
+      <c r="M94" s="292"/>
+      <c r="N94" s="290" t="s">
         <v>180</v>
       </c>
-      <c r="O94" s="277"/>
-      <c r="P94" s="277"/>
-      <c r="Q94" s="277"/>
-      <c r="R94" s="277"/>
-      <c r="S94" s="277"/>
-      <c r="T94" s="277" t="s">
+      <c r="O94" s="290"/>
+      <c r="P94" s="290"/>
+      <c r="Q94" s="290"/>
+      <c r="R94" s="290"/>
+      <c r="S94" s="290"/>
+      <c r="T94" s="290" t="s">
         <v>181</v>
       </c>
-      <c r="U94" s="277"/>
-      <c r="V94" s="277"/>
-      <c r="W94" s="277" t="s">
+      <c r="U94" s="290"/>
+      <c r="V94" s="290"/>
+      <c r="W94" s="290" t="s">
         <v>182</v>
       </c>
-      <c r="X94" s="277"/>
-      <c r="Y94" s="277"/>
+      <c r="X94" s="290"/>
+      <c r="Y94" s="290"/>
     </row>
     <row r="95" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A95" s="247" t="s">
@@ -6725,11 +6733,11 @@
       <c r="J95" s="272">
         <v>1249</v>
       </c>
-      <c r="K95" s="280" t="s">
+      <c r="K95" s="293" t="s">
         <v>237</v>
       </c>
-      <c r="L95" s="280"/>
-      <c r="M95" s="280"/>
+      <c r="L95" s="294"/>
+      <c r="M95" s="295"/>
       <c r="N95" s="272">
         <v>1157</v>
       </c>
@@ -6798,11 +6806,11 @@
       <c r="J96" s="272">
         <v>936</v>
       </c>
-      <c r="K96" s="277" t="s">
-        <v>236</v>
-      </c>
-      <c r="L96" s="277"/>
-      <c r="M96" s="277"/>
+      <c r="K96" s="290" t="s">
+        <v>237</v>
+      </c>
+      <c r="L96" s="290"/>
+      <c r="M96" s="290"/>
       <c r="N96" s="272">
         <v>842</v>
       </c>
@@ -6871,11 +6879,11 @@
       <c r="J97" s="272">
         <v>1250</v>
       </c>
-      <c r="K97" s="277" t="s">
+      <c r="K97" s="290" t="s">
         <v>236</v>
       </c>
-      <c r="L97" s="277"/>
-      <c r="M97" s="277"/>
+      <c r="L97" s="290"/>
+      <c r="M97" s="290"/>
       <c r="N97" s="272">
         <v>1158</v>
       </c>
@@ -6944,11 +6952,11 @@
       <c r="J98" s="272">
         <v>937</v>
       </c>
-      <c r="K98" s="277" t="s">
+      <c r="K98" s="290" t="s">
         <v>236</v>
       </c>
-      <c r="L98" s="277"/>
-      <c r="M98" s="277"/>
+      <c r="L98" s="290"/>
+      <c r="M98" s="290"/>
       <c r="N98" s="272">
         <v>843</v>
       </c>
@@ -7017,11 +7025,11 @@
       <c r="J99" s="272">
         <v>1251</v>
       </c>
-      <c r="K99" s="277" t="s">
+      <c r="K99" s="290" t="s">
         <v>236</v>
       </c>
-      <c r="L99" s="277"/>
-      <c r="M99" s="277"/>
+      <c r="L99" s="290"/>
+      <c r="M99" s="290"/>
       <c r="N99" s="272">
         <v>1159</v>
       </c>
@@ -7090,11 +7098,11 @@
       <c r="J100" s="272">
         <v>938</v>
       </c>
-      <c r="K100" s="277" t="s">
+      <c r="K100" s="290" t="s">
         <v>236</v>
       </c>
-      <c r="L100" s="277"/>
-      <c r="M100" s="277"/>
+      <c r="L100" s="290"/>
+      <c r="M100" s="290"/>
       <c r="N100" s="272">
         <v>844</v>
       </c>
@@ -7163,11 +7171,11 @@
       <c r="J101" s="272">
         <v>1252</v>
       </c>
-      <c r="K101" s="277" t="s">
+      <c r="K101" s="290" t="s">
         <v>236</v>
       </c>
-      <c r="L101" s="277"/>
-      <c r="M101" s="277"/>
+      <c r="L101" s="290"/>
+      <c r="M101" s="290"/>
       <c r="N101" s="272">
         <v>1160</v>
       </c>
@@ -7236,11 +7244,11 @@
       <c r="J102" s="272">
         <v>939</v>
       </c>
-      <c r="K102" s="277" t="s">
+      <c r="K102" s="290" t="s">
         <v>236</v>
       </c>
-      <c r="L102" s="277"/>
-      <c r="M102" s="277"/>
+      <c r="L102" s="290"/>
+      <c r="M102" s="290"/>
       <c r="N102" s="272">
         <v>845</v>
       </c>
@@ -7309,11 +7317,11 @@
       <c r="J103" s="272">
         <v>1253</v>
       </c>
-      <c r="K103" s="277" t="s">
+      <c r="K103" s="290" t="s">
         <v>236</v>
       </c>
-      <c r="L103" s="277"/>
-      <c r="M103" s="277"/>
+      <c r="L103" s="290"/>
+      <c r="M103" s="290"/>
       <c r="N103" s="272">
         <v>1161</v>
       </c>
@@ -7382,11 +7390,11 @@
       <c r="J104" s="272">
         <v>940</v>
       </c>
-      <c r="K104" s="277" t="s">
+      <c r="K104" s="290" t="s">
         <v>236</v>
       </c>
-      <c r="L104" s="277"/>
-      <c r="M104" s="277"/>
+      <c r="L104" s="290"/>
+      <c r="M104" s="290"/>
       <c r="N104" s="272">
         <v>846</v>
       </c>
@@ -7455,11 +7463,11 @@
       <c r="J105" s="272">
         <v>1254</v>
       </c>
-      <c r="K105" s="277" t="s">
+      <c r="K105" s="290" t="s">
         <v>236</v>
       </c>
-      <c r="L105" s="277"/>
-      <c r="M105" s="277"/>
+      <c r="L105" s="290"/>
+      <c r="M105" s="290"/>
       <c r="N105" s="272">
         <v>1162</v>
       </c>
@@ -7528,11 +7536,11 @@
       <c r="J106" s="272">
         <v>941</v>
       </c>
-      <c r="K106" s="277" t="s">
+      <c r="K106" s="290" t="s">
         <v>236</v>
       </c>
-      <c r="L106" s="277"/>
-      <c r="M106" s="277"/>
+      <c r="L106" s="290"/>
+      <c r="M106" s="290"/>
       <c r="N106" s="272">
         <v>847</v>
       </c>
@@ -7601,11 +7609,11 @@
       <c r="J107" s="272">
         <v>1255</v>
       </c>
-      <c r="K107" s="277" t="s">
+      <c r="K107" s="290" t="s">
         <v>236</v>
       </c>
-      <c r="L107" s="277"/>
-      <c r="M107" s="277"/>
+      <c r="L107" s="290"/>
+      <c r="M107" s="290"/>
       <c r="N107" s="272">
         <v>1163</v>
       </c>
@@ -7674,11 +7682,11 @@
       <c r="J108" s="272">
         <v>942</v>
       </c>
-      <c r="K108" s="277" t="s">
+      <c r="K108" s="290" t="s">
         <v>236</v>
       </c>
-      <c r="L108" s="277"/>
-      <c r="M108" s="277"/>
+      <c r="L108" s="290"/>
+      <c r="M108" s="290"/>
       <c r="N108" s="272">
         <v>848</v>
       </c>
@@ -7747,11 +7755,11 @@
       <c r="J109" s="272">
         <v>1256</v>
       </c>
-      <c r="K109" s="277" t="s">
+      <c r="K109" s="290" t="s">
         <v>235</v>
       </c>
-      <c r="L109" s="277"/>
-      <c r="M109" s="277"/>
+      <c r="L109" s="290"/>
+      <c r="M109" s="290"/>
       <c r="N109" s="272">
         <v>1164</v>
       </c>
@@ -7793,11 +7801,11 @@
       <c r="B110" t="s">
         <v>234</v>
       </c>
-      <c r="K110" s="278" t="s">
+      <c r="K110" s="291" t="s">
         <v>243</v>
       </c>
-      <c r="L110" s="278"/>
-      <c r="M110" s="278"/>
+      <c r="L110" s="291"/>
+      <c r="M110" s="291"/>
       <c r="N110" t="s">
         <v>242</v>
       </c>
@@ -7950,26 +7958,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="J66:J71"/>
-    <mergeCell ref="B1:M1"/>
-    <mergeCell ref="M2:O3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="R66:S66"/>
-    <mergeCell ref="T66:U66"/>
-    <mergeCell ref="X67:X71"/>
-    <mergeCell ref="W94:Y94"/>
-    <mergeCell ref="T94:V94"/>
-    <mergeCell ref="N94:S94"/>
-    <mergeCell ref="K96:M96"/>
-    <mergeCell ref="K97:M97"/>
-    <mergeCell ref="K98:M98"/>
-    <mergeCell ref="K99:M99"/>
-    <mergeCell ref="P66:Q66"/>
     <mergeCell ref="K106:M106"/>
     <mergeCell ref="K107:M107"/>
     <mergeCell ref="K110:M110"/>
@@ -7986,10 +7974,30 @@
     <mergeCell ref="K109:M109"/>
     <mergeCell ref="K108:M108"/>
     <mergeCell ref="K95:M95"/>
+    <mergeCell ref="K96:M96"/>
+    <mergeCell ref="K97:M97"/>
+    <mergeCell ref="K98:M98"/>
+    <mergeCell ref="K99:M99"/>
+    <mergeCell ref="P66:Q66"/>
+    <mergeCell ref="R66:S66"/>
+    <mergeCell ref="T66:U66"/>
+    <mergeCell ref="X67:X71"/>
+    <mergeCell ref="W94:Y94"/>
+    <mergeCell ref="T94:V94"/>
+    <mergeCell ref="N94:S94"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="J66:J71"/>
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="M2:O3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K7:L7"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="30" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="40" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>